<commit_message>
Added newest data, removed old data
</commit_message>
<xml_diff>
--- a/Auswertung_Hauptstudie/data_masterstudie_filtered.xlsx
+++ b/Auswertung_Hauptstudie/data_masterstudie_filtered.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR149"/>
+  <dimension ref="A1:AS160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,10 +649,15 @@
           <t>RISK_TOTAL</t>
         </is>
       </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>RISK_TOLERANCE_TOTAL</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -775,10 +780,13 @@
       <c r="AR2" t="n">
         <v>46.2</v>
       </c>
+      <c r="AS2" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -810,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="M3" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="N3" t="n">
         <v>4</v>
@@ -901,10 +909,13 @@
       <c r="AR3" t="n">
         <v>20</v>
       </c>
+      <c r="AS3" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -1019,10 +1030,13 @@
       <c r="AR4" t="n">
         <v>28</v>
       </c>
+      <c r="AS4" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -1137,10 +1151,13 @@
       <c r="AR5" t="n">
         <v>50</v>
       </c>
+      <c r="AS5" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -1263,10 +1280,13 @@
       <c r="AR6" t="n">
         <v>50</v>
       </c>
+      <c r="AS6" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>2</v>
@@ -1316,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="S7" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
@@ -1372,7 +1392,7 @@
         <v>3</v>
       </c>
       <c r="AM7" t="n">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="AN7" t="n">
         <v>1</v>
@@ -1388,11 +1408,14 @@
       </c>
       <c r="AR7" t="n">
         <v>0</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>3</v>
@@ -1507,10 +1530,13 @@
       <c r="AR8" t="n">
         <v>50</v>
       </c>
+      <c r="AS8" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
@@ -1633,10 +1659,13 @@
       <c r="AR9" t="n">
         <v>25.9</v>
       </c>
+      <c r="AS9" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>3</v>
@@ -1763,10 +1792,13 @@
       <c r="AR10" t="n">
         <v>5</v>
       </c>
+      <c r="AS10" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>4</v>
@@ -1870,7 +1902,7 @@
         <v>2</v>
       </c>
       <c r="AO11" t="n">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="AP11" t="n">
         <v>1</v>
@@ -1880,11 +1912,14 @@
       </c>
       <c r="AR11" t="n">
         <v>50</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>5</v>
@@ -1988,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="AO12" t="n">
-        <v>748</v>
+        <v>692</v>
       </c>
       <c r="AP12" t="n">
         <v>1</v>
@@ -1998,11 +2033,14 @@
       </c>
       <c r="AR12" t="n">
         <v>50</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>6</v>
@@ -2125,10 +2163,13 @@
       <c r="AR13" t="n">
         <v>60</v>
       </c>
+      <c r="AS13" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>5</v>
@@ -2251,10 +2292,13 @@
       <c r="AR14" t="n">
         <v>29.6</v>
       </c>
+      <c r="AS14" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>6</v>
@@ -2377,10 +2421,13 @@
       <c r="AR15" t="n">
         <v>12.9</v>
       </c>
+      <c r="AS15" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>6</v>
@@ -2495,10 +2542,13 @@
       <c r="AR16" t="n">
         <v>25</v>
       </c>
+      <c r="AS16" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B17" t="n">
         <v>7</v>
@@ -2613,10 +2663,13 @@
       <c r="AR17" t="n">
         <v>15</v>
       </c>
+      <c r="AS17" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>7</v>
@@ -2728,7 +2781,7 @@
         <v>1</v>
       </c>
       <c r="AO18" t="n">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AP18" t="n">
         <v>1</v>
@@ -2738,11 +2791,14 @@
       </c>
       <c r="AR18" t="n">
         <v>25</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B19" t="n">
         <v>7</v>
@@ -2865,10 +2921,13 @@
       <c r="AR19" t="n">
         <v>35.6</v>
       </c>
+      <c r="AS19" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B20" t="n">
         <v>8</v>
@@ -2977,10 +3036,10 @@
         <v>1</v>
       </c>
       <c r="AN20" t="n">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="AO20" t="n">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AP20" t="n">
         <v>1</v>
@@ -2990,11 +3049,14 @@
       </c>
       <c r="AR20" t="n">
         <v>49.4</v>
+      </c>
+      <c r="AS20" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>8</v>
@@ -3098,7 +3160,7 @@
         <v>3</v>
       </c>
       <c r="AO21" t="n">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AP21" t="n">
         <v>1</v>
@@ -3108,11 +3170,14 @@
       </c>
       <c r="AR21" t="n">
         <v>70</v>
+      </c>
+      <c r="AS21" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>8</v>
@@ -3224,7 +3289,7 @@
         <v>3</v>
       </c>
       <c r="AO22" t="n">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="AP22" t="n">
         <v>1</v>
@@ -3234,11 +3299,14 @@
       </c>
       <c r="AR22" t="n">
         <v>30.1</v>
+      </c>
+      <c r="AS22" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>9</v>
@@ -3342,7 +3410,7 @@
         <v>3</v>
       </c>
       <c r="AO23" t="n">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AP23" t="n">
         <v>1</v>
@@ -3352,11 +3420,14 @@
       </c>
       <c r="AR23" t="n">
         <v>100</v>
+      </c>
+      <c r="AS23" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B24" t="n">
         <v>9</v>
@@ -3479,10 +3550,13 @@
       <c r="AR24" t="n">
         <v>10</v>
       </c>
+      <c r="AS24" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B25" t="n">
         <v>9</v>
@@ -3518,7 +3592,7 @@
         <v>5</v>
       </c>
       <c r="M25" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="N25" t="n">
         <v>4</v>
@@ -3598,7 +3672,7 @@
         <v>1</v>
       </c>
       <c r="AO25" t="n">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="AP25" t="n">
         <v>1</v>
@@ -3608,11 +3682,14 @@
       </c>
       <c r="AR25" t="n">
         <v>31.4</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B26" t="n">
         <v>10</v>
@@ -3644,7 +3721,7 @@
         <v>4</v>
       </c>
       <c r="M26" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="N26" t="n">
         <v>2</v>
@@ -3727,10 +3804,13 @@
       <c r="AR26" t="n">
         <v>0</v>
       </c>
+      <c r="AS26" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>10</v>
@@ -3853,10 +3933,13 @@
       <c r="AR27" t="n">
         <v>61.90000000000001</v>
       </c>
+      <c r="AS27" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B28" t="n">
         <v>11</v>
@@ -3979,10 +4062,13 @@
       <c r="AR28" t="n">
         <v>72.7</v>
       </c>
+      <c r="AS28" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B29" t="n">
         <v>11</v>
@@ -4086,7 +4172,7 @@
         <v>1</v>
       </c>
       <c r="AO29" t="n">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="AP29" t="n">
         <v>1</v>
@@ -4096,11 +4182,14 @@
       </c>
       <c r="AR29" t="n">
         <v>25</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B30" t="n">
         <v>11</v>
@@ -4231,10 +4320,13 @@
       <c r="AR30" t="n">
         <v>0</v>
       </c>
+      <c r="AS30" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B31" t="n">
         <v>12</v>
@@ -4338,7 +4430,7 @@
         <v>1</v>
       </c>
       <c r="AO31" t="n">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="AP31" t="n">
         <v>1</v>
@@ -4348,11 +4440,14 @@
       </c>
       <c r="AR31" t="n">
         <v>10</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>12</v>
@@ -4475,10 +4570,13 @@
       <c r="AR32" t="n">
         <v>55</v>
       </c>
+      <c r="AS32" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B33" t="n">
         <v>13</v>
@@ -4590,7 +4688,7 @@
         <v>1</v>
       </c>
       <c r="AO33" t="n">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="AP33" t="n">
         <v>1</v>
@@ -4600,11 +4698,14 @@
       </c>
       <c r="AR33" t="n">
         <v>10</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B34" t="n">
         <v>13</v>
@@ -4719,10 +4820,13 @@
       <c r="AR34" t="n">
         <v>10</v>
       </c>
+      <c r="AS34" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B35" t="n">
         <v>13</v>
@@ -4838,7 +4942,7 @@
         <v>1</v>
       </c>
       <c r="AO35" t="n">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AP35" t="n">
         <v>1</v>
@@ -4848,11 +4952,14 @@
       </c>
       <c r="AR35" t="n">
         <v>21.2</v>
+      </c>
+      <c r="AS35" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B36" t="n">
         <v>14</v>
@@ -4975,10 +5082,13 @@
       <c r="AR36" t="n">
         <v>0.3</v>
       </c>
+      <c r="AS36" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B37" t="n">
         <v>15</v>
@@ -5101,10 +5211,13 @@
       <c r="AR37" t="n">
         <v>18.7</v>
       </c>
+      <c r="AS37" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B38" t="n">
         <v>14</v>
@@ -5216,7 +5329,7 @@
         <v>1</v>
       </c>
       <c r="AO38" t="n">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="AP38" t="n">
         <v>1</v>
@@ -5226,11 +5339,14 @@
       </c>
       <c r="AR38" t="n">
         <v>39.09999999999999</v>
+      </c>
+      <c r="AS38" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B39" t="n">
         <v>15</v>
@@ -5353,10 +5469,13 @@
       <c r="AR39" t="n">
         <v>30</v>
       </c>
+      <c r="AS39" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B40" t="n">
         <v>17</v>
@@ -5479,10 +5598,13 @@
       <c r="AR40" t="n">
         <v>0</v>
       </c>
+      <c r="AS40" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B41" t="n">
         <v>17</v>
@@ -5605,10 +5727,13 @@
       <c r="AR41" t="n">
         <v>57.2</v>
       </c>
+      <c r="AS41" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B42" t="n">
         <v>17</v>
@@ -5658,7 +5783,7 @@
         <v>1</v>
       </c>
       <c r="S42" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="T42" t="n">
         <v>100</v>
@@ -5723,10 +5848,13 @@
       <c r="AR42" t="n">
         <v>100</v>
       </c>
+      <c r="AS42" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B43" t="n">
         <v>18</v>
@@ -5841,10 +5969,13 @@
       <c r="AR43" t="n">
         <v>30</v>
       </c>
+      <c r="AS43" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B44" t="n">
         <v>18</v>
@@ -5967,10 +6098,13 @@
       <c r="AR44" t="n">
         <v>49</v>
       </c>
+      <c r="AS44" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B45" t="n">
         <v>19</v>
@@ -6093,10 +6227,13 @@
       <c r="AR45" t="n">
         <v>27.2</v>
       </c>
+      <c r="AS45" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B46" t="n">
         <v>19</v>
@@ -6131,7 +6268,7 @@
         <v>4</v>
       </c>
       <c r="N46" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="O46" t="n">
         <v>5</v>
@@ -6182,7 +6319,7 @@
         <v>2</v>
       </c>
       <c r="AI46" t="n">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="AJ46" t="n">
         <v>1</v>
@@ -6200,7 +6337,7 @@
         <v>2</v>
       </c>
       <c r="AO46" t="n">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AP46" t="n">
         <v>1</v>
@@ -6210,11 +6347,14 @@
       </c>
       <c r="AR46" t="n">
         <v>5</v>
+      </c>
+      <c r="AS46" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>20</v>
@@ -6318,7 +6458,7 @@
         <v>2</v>
       </c>
       <c r="AO47" t="n">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AP47" t="n">
         <v>1</v>
@@ -6328,11 +6468,14 @@
       </c>
       <c r="AR47" t="n">
         <v>90</v>
+      </c>
+      <c r="AS47" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B48" t="n">
         <v>20</v>
@@ -6455,10 +6598,13 @@
       <c r="AR48" t="n">
         <v>1</v>
       </c>
+      <c r="AS48" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B49" t="n">
         <v>20</v>
@@ -6490,7 +6636,7 @@
         <v>5</v>
       </c>
       <c r="M49" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="N49" t="n">
         <v>5</v>
@@ -6581,10 +6727,13 @@
       <c r="AR49" t="n">
         <v>5</v>
       </c>
+      <c r="AS49" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B50" t="n">
         <v>21</v>
@@ -6634,7 +6783,7 @@
         <v>1</v>
       </c>
       <c r="S50" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="T50" t="n">
         <v>10</v>
@@ -6699,10 +6848,13 @@
       <c r="AR50" t="n">
         <v>10</v>
       </c>
+      <c r="AS50" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B51" t="n">
         <v>21</v>
@@ -6825,10 +6977,13 @@
       <c r="AR51" t="n">
         <v>45</v>
       </c>
+      <c r="AS51" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B52" t="n">
         <v>22</v>
@@ -6951,10 +7106,13 @@
       <c r="AR52" t="n">
         <v>32.5</v>
       </c>
+      <c r="AS52" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B53" t="n">
         <v>22</v>
@@ -7077,10 +7235,13 @@
       <c r="AR53" t="n">
         <v>33.9</v>
       </c>
+      <c r="AS53" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B54" t="n">
         <v>22</v>
@@ -7195,10 +7356,13 @@
       <c r="AR54" t="n">
         <v>50</v>
       </c>
+      <c r="AS54" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B55" t="n">
         <v>23</v>
@@ -7321,10 +7485,13 @@
       <c r="AR55" t="n">
         <v>6.199999999999999</v>
       </c>
+      <c r="AS55" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B56" t="n">
         <v>23</v>
@@ -7439,10 +7606,13 @@
       <c r="AR56" t="n">
         <v>43</v>
       </c>
+      <c r="AS56" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B57" t="n">
         <v>23</v>
@@ -7565,10 +7735,13 @@
       <c r="AR57" t="n">
         <v>37</v>
       </c>
+      <c r="AS57" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B58" t="n">
         <v>24</v>
@@ -7691,10 +7864,13 @@
       <c r="AR58" t="n">
         <v>5.600000000000001</v>
       </c>
+      <c r="AS58" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B59" t="n">
         <v>24</v>
@@ -7817,10 +7993,13 @@
       <c r="AR59" t="n">
         <v>40</v>
       </c>
+      <c r="AS59" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B60" t="n">
         <v>24</v>
@@ -7924,7 +8103,7 @@
         <v>2</v>
       </c>
       <c r="AO60" t="n">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AP60" t="n">
         <v>1</v>
@@ -7934,11 +8113,14 @@
       </c>
       <c r="AR60" t="n">
         <v>37</v>
+      </c>
+      <c r="AS60" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B61" t="n">
         <v>25</v>
@@ -8032,7 +8214,7 @@
         <v>1</v>
       </c>
       <c r="AI61" t="n">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="AJ61" t="n">
         <v>1</v>
@@ -8060,11 +8242,14 @@
       </c>
       <c r="AR61" t="n">
         <v>5</v>
+      </c>
+      <c r="AS61" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B62" t="n">
         <v>25</v>
@@ -8187,10 +8372,13 @@
       <c r="AR62" t="n">
         <v>9.800000000000001</v>
       </c>
+      <c r="AS62" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="B63" t="n">
         <v>26</v>
@@ -8313,10 +8501,13 @@
       <c r="AR63" t="n">
         <v>52</v>
       </c>
+      <c r="AS63" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B64" t="n">
         <v>26</v>
@@ -8439,10 +8630,13 @@
       <c r="AR64" t="n">
         <v>0</v>
       </c>
+      <c r="AS64" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B65" t="n">
         <v>26</v>
@@ -8557,10 +8751,13 @@
       <c r="AR65" t="n">
         <v>27</v>
       </c>
+      <c r="AS65" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B66" t="n">
         <v>27</v>
@@ -8672,7 +8869,7 @@
         <v>3</v>
       </c>
       <c r="AO66" t="n">
-        <v>652</v>
+        <v>394</v>
       </c>
       <c r="AP66" t="n">
         <v>1</v>
@@ -8682,11 +8879,14 @@
       </c>
       <c r="AR66" t="n">
         <v>69.19999999999999</v>
+      </c>
+      <c r="AS66" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B67" t="n">
         <v>27</v>
@@ -8801,10 +9001,13 @@
       <c r="AR67" t="n">
         <v>0</v>
       </c>
+      <c r="AS67" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B68" t="n">
         <v>27</v>
@@ -8927,10 +9130,13 @@
       <c r="AR68" t="n">
         <v>82.59999999999999</v>
       </c>
+      <c r="AS68" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B69" t="n">
         <v>28</v>
@@ -9042,7 +9248,7 @@
         <v>2</v>
       </c>
       <c r="AO69" t="n">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AP69" t="n">
         <v>1</v>
@@ -9052,11 +9258,14 @@
       </c>
       <c r="AR69" t="n">
         <v>40</v>
+      </c>
+      <c r="AS69" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B70" t="n">
         <v>28</v>
@@ -9171,10 +9380,13 @@
       <c r="AR70" t="n">
         <v>25</v>
       </c>
+      <c r="AS70" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B71" t="n">
         <v>28</v>
@@ -9297,10 +9509,13 @@
       <c r="AR71" t="n">
         <v>10</v>
       </c>
+      <c r="AS71" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B72" t="n">
         <v>29</v>
@@ -9412,7 +9627,7 @@
         <v>2</v>
       </c>
       <c r="AO72" t="n">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="AP72" t="n">
         <v>1</v>
@@ -9422,11 +9637,14 @@
       </c>
       <c r="AR72" t="n">
         <v>0</v>
+      </c>
+      <c r="AS72" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B73" t="n">
         <v>29</v>
@@ -9541,10 +9759,13 @@
       <c r="AR73" t="n">
         <v>31</v>
       </c>
+      <c r="AS73" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B74" t="n">
         <v>29</v>
@@ -9667,10 +9888,13 @@
       <c r="AR74" t="n">
         <v>5</v>
       </c>
+      <c r="AS74" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="B75" t="n">
         <v>30</v>
@@ -9793,10 +10017,13 @@
       <c r="AR75" t="n">
         <v>40.5</v>
       </c>
+      <c r="AS75" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B76" t="n">
         <v>30</v>
@@ -9919,10 +10146,13 @@
       <c r="AR76" t="n">
         <v>30</v>
       </c>
+      <c r="AS76" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="B77" t="n">
         <v>30</v>
@@ -10037,10 +10267,13 @@
       <c r="AR77" t="n">
         <v>65</v>
       </c>
+      <c r="AS77" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B78" t="n">
         <v>31</v>
@@ -10155,10 +10388,13 @@
       <c r="AR78" t="n">
         <v>0</v>
       </c>
+      <c r="AS78" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B79" t="n">
         <v>31</v>
@@ -10258,7 +10494,7 @@
         <v>1</v>
       </c>
       <c r="AK79" t="n">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="AL79" t="n">
         <v>2</v>
@@ -10270,7 +10506,7 @@
         <v>2</v>
       </c>
       <c r="AO79" t="n">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="AP79" t="n">
         <v>1</v>
@@ -10280,11 +10516,14 @@
       </c>
       <c r="AR79" t="n">
         <v>0</v>
+      </c>
+      <c r="AS79" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B80" t="n">
         <v>32</v>
@@ -10407,10 +10646,13 @@
       <c r="AR80" t="n">
         <v>37.3</v>
       </c>
+      <c r="AS80" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="B81" t="n">
         <v>32</v>
@@ -10533,10 +10775,13 @@
       <c r="AR81" t="n">
         <v>0</v>
       </c>
+      <c r="AS81" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B82" t="n">
         <v>33</v>
@@ -10659,10 +10904,13 @@
       <c r="AR82" t="n">
         <v>15.2</v>
       </c>
+      <c r="AS82" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B83" t="n">
         <v>33</v>
@@ -10766,7 +11014,7 @@
         <v>2</v>
       </c>
       <c r="AO83" t="n">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AP83" t="n">
         <v>1</v>
@@ -10776,11 +11024,14 @@
       </c>
       <c r="AR83" t="n">
         <v>10</v>
+      </c>
+      <c r="AS83" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B84" t="n">
         <v>33</v>
@@ -10812,7 +11063,7 @@
         <v>5</v>
       </c>
       <c r="M84" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="N84" t="n">
         <v>2</v>
@@ -10903,10 +11154,13 @@
       <c r="AR84" t="n">
         <v>7.6</v>
       </c>
+      <c r="AS84" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B85" t="n">
         <v>34</v>
@@ -11029,10 +11283,13 @@
       <c r="AR85" t="n">
         <v>5</v>
       </c>
+      <c r="AS85" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B86" t="n">
         <v>34</v>
@@ -11067,7 +11324,7 @@
         <v>2</v>
       </c>
       <c r="N86" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="O86" t="n">
         <v>5</v>
@@ -11155,10 +11412,13 @@
       <c r="AR86" t="n">
         <v>33.5</v>
       </c>
+      <c r="AS86" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B87" t="n">
         <v>34</v>
@@ -11273,10 +11533,13 @@
       <c r="AR87" t="n">
         <v>20</v>
       </c>
+      <c r="AS87" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B88" t="n">
         <v>35</v>
@@ -11391,10 +11654,13 @@
       <c r="AR88" t="n">
         <v>10</v>
       </c>
+      <c r="AS88" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="B89" t="n">
         <v>35</v>
@@ -11517,10 +11783,13 @@
       <c r="AR89" t="n">
         <v>53.3</v>
       </c>
+      <c r="AS89" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="B90" t="n">
         <v>35</v>
@@ -11643,10 +11912,13 @@
       <c r="AR90" t="n">
         <v>8.899999999999999</v>
       </c>
+      <c r="AS90" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="B91" t="n">
         <v>36</v>
@@ -11761,10 +12033,13 @@
       <c r="AR91" t="n">
         <v>20</v>
       </c>
+      <c r="AS91" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="B92" t="n">
         <v>36</v>
@@ -11887,10 +12162,13 @@
       <c r="AR92" t="n">
         <v>20</v>
       </c>
+      <c r="AS92" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="B93" t="n">
         <v>37</v>
@@ -12002,7 +12280,7 @@
         <v>2</v>
       </c>
       <c r="AO93" t="n">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AP93" t="n">
         <v>1</v>
@@ -12012,11 +12290,14 @@
       </c>
       <c r="AR93" t="n">
         <v>52</v>
+      </c>
+      <c r="AS93" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="B94" t="n">
         <v>37</v>
@@ -12094,7 +12375,7 @@
         <v>2</v>
       </c>
       <c r="AE94" t="n">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="AF94" t="n">
         <v>1</v>
@@ -12134,11 +12415,14 @@
       </c>
       <c r="AR94" t="n">
         <v>33</v>
+      </c>
+      <c r="AS94" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="B95" t="n">
         <v>37</v>
@@ -12250,7 +12534,7 @@
         <v>1</v>
       </c>
       <c r="AO95" t="n">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="AP95" t="n">
         <v>1</v>
@@ -12260,11 +12544,14 @@
       </c>
       <c r="AR95" t="n">
         <v>31.1</v>
+      </c>
+      <c r="AS95" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="B96" t="n">
         <v>38</v>
@@ -12387,10 +12674,13 @@
       <c r="AR96" t="n">
         <v>20.7</v>
       </c>
+      <c r="AS96" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="B97" t="n">
         <v>38</v>
@@ -12505,10 +12795,13 @@
       <c r="AR97" t="n">
         <v>28</v>
       </c>
+      <c r="AS97" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="B98" t="n">
         <v>39</v>
@@ -12631,10 +12924,13 @@
       <c r="AR98" t="n">
         <v>80.09999999999999</v>
       </c>
+      <c r="AS98" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="B99" t="n">
         <v>39</v>
@@ -12757,10 +13053,13 @@
       <c r="AR99" t="n">
         <v>83.60000000000001</v>
       </c>
+      <c r="AS99" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B100" t="n">
         <v>40</v>
@@ -12872,7 +13171,7 @@
         <v>2</v>
       </c>
       <c r="AO100" t="n">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AP100" t="n">
         <v>1</v>
@@ -12882,11 +13181,14 @@
       </c>
       <c r="AR100" t="n">
         <v>15</v>
+      </c>
+      <c r="AS100" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B101" t="n">
         <v>40</v>
@@ -13009,10 +13311,13 @@
       <c r="AR101" t="n">
         <v>0</v>
       </c>
+      <c r="AS101" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B102" t="n">
         <v>40</v>
@@ -13127,10 +13432,13 @@
       <c r="AR102" t="n">
         <v>34</v>
       </c>
+      <c r="AS102" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B103" t="n">
         <v>41</v>
@@ -13234,7 +13542,7 @@
         <v>2</v>
       </c>
       <c r="AO103" t="n">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="AP103" t="n">
         <v>1</v>
@@ -13244,11 +13552,14 @@
       </c>
       <c r="AR103" t="n">
         <v>30</v>
+      </c>
+      <c r="AS103" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="B104" t="n">
         <v>41</v>
@@ -13342,7 +13653,7 @@
         <v>2</v>
       </c>
       <c r="AI104" t="n">
-        <v>-9</v>
+        <v>1</v>
       </c>
       <c r="AJ104" t="n">
         <v>1</v>
@@ -13370,11 +13681,14 @@
       </c>
       <c r="AR104" t="n">
         <v>34.1</v>
+      </c>
+      <c r="AS104" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="B105" t="n">
         <v>41</v>
@@ -13497,10 +13811,13 @@
       <c r="AR105" t="n">
         <v>100</v>
       </c>
+      <c r="AS105" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="B106" t="n">
         <v>42</v>
@@ -13623,10 +13940,13 @@
       <c r="AR106" t="n">
         <v>40</v>
       </c>
+      <c r="AS106" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="B107" t="n">
         <v>42</v>
@@ -13741,10 +14061,13 @@
       <c r="AR107" t="n">
         <v>0</v>
       </c>
+      <c r="AS107" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="B108" t="n">
         <v>42</v>
@@ -13867,10 +14190,13 @@
       <c r="AR108" t="n">
         <v>1.5</v>
       </c>
+      <c r="AS108" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="B109" t="n">
         <v>43</v>
@@ -13993,10 +14319,13 @@
       <c r="AR109" t="n">
         <v>48.3</v>
       </c>
+      <c r="AS109" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="B110" t="n">
         <v>43</v>
@@ -14119,10 +14448,13 @@
       <c r="AR110" t="n">
         <v>50</v>
       </c>
+      <c r="AS110" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="B111" t="n">
         <v>43</v>
@@ -14237,10 +14569,13 @@
       <c r="AR111" t="n">
         <v>0</v>
       </c>
+      <c r="AS111" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="B112" t="n">
         <v>44</v>
@@ -14355,10 +14690,13 @@
       <c r="AR112" t="n">
         <v>20</v>
       </c>
+      <c r="AS112" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="B113" t="n">
         <v>44</v>
@@ -14481,10 +14819,13 @@
       <c r="AR113" t="n">
         <v>0.5</v>
       </c>
+      <c r="AS113" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B114" t="n">
         <v>44</v>
@@ -14607,10 +14948,13 @@
       <c r="AR114" t="n">
         <v>29</v>
       </c>
+      <c r="AS114" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B115" t="n">
         <v>45</v>
@@ -14733,10 +15077,13 @@
       <c r="AR115" t="n">
         <v>20.6</v>
       </c>
+      <c r="AS115" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="B116" t="n">
         <v>45</v>
@@ -14851,10 +15198,13 @@
       <c r="AR116" t="n">
         <v>20</v>
       </c>
+      <c r="AS116" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B117" t="n">
         <v>45</v>
@@ -14977,10 +15327,13 @@
       <c r="AR117" t="n">
         <v>30.3</v>
       </c>
+      <c r="AS117" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="B118" t="n">
         <v>46</v>
@@ -15095,10 +15448,13 @@
       <c r="AR118" t="n">
         <v>20</v>
       </c>
+      <c r="AS118" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="B119" t="n">
         <v>46</v>
@@ -15221,10 +15577,13 @@
       <c r="AR119" t="n">
         <v>35</v>
       </c>
+      <c r="AS119" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="B120" t="n">
         <v>47</v>
@@ -15339,10 +15698,13 @@
       <c r="AR120" t="n">
         <v>20</v>
       </c>
+      <c r="AS120" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="B121" t="n">
         <v>47</v>
@@ -15465,10 +15827,13 @@
       <c r="AR121" t="n">
         <v>8.6</v>
       </c>
+      <c r="AS121" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="B122" t="n">
         <v>47</v>
@@ -15591,10 +15956,13 @@
       <c r="AR122" t="n">
         <v>20.1</v>
       </c>
+      <c r="AS122" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="B123" t="n">
         <v>48</v>
@@ -15717,10 +16085,13 @@
       <c r="AR123" t="n">
         <v>3.6</v>
       </c>
+      <c r="AS123" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="B124" t="n">
         <v>48</v>
@@ -15835,10 +16206,13 @@
       <c r="AR124" t="n">
         <v>20</v>
       </c>
+      <c r="AS124" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="B125" t="n">
         <v>48</v>
@@ -15961,10 +16335,13 @@
       <c r="AR125" t="n">
         <v>29.6</v>
       </c>
+      <c r="AS125" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="B126" t="n">
         <v>49</v>
@@ -16079,10 +16456,13 @@
       <c r="AR126" t="n">
         <v>20</v>
       </c>
+      <c r="AS126" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="B127" t="n">
         <v>49</v>
@@ -16205,10 +16585,13 @@
       <c r="AR127" t="n">
         <v>100</v>
       </c>
+      <c r="AS127" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="B128" t="n">
         <v>49</v>
@@ -16335,10 +16718,13 @@
       <c r="AR128" t="n">
         <v>65</v>
       </c>
+      <c r="AS128" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B129" t="n">
         <v>50</v>
@@ -16453,10 +16839,13 @@
       <c r="AR129" t="n">
         <v>30</v>
       </c>
+      <c r="AS129" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B130" t="n">
         <v>50</v>
@@ -16579,10 +16968,13 @@
       <c r="AR130" t="n">
         <v>40.09999999999999</v>
       </c>
+      <c r="AS130" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="B131" t="n">
         <v>51</v>
@@ -16697,10 +17089,13 @@
       <c r="AR131" t="n">
         <v>20</v>
       </c>
+      <c r="AS131" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="B132" t="n">
         <v>51</v>
@@ -16823,10 +17218,13 @@
       <c r="AR132" t="n">
         <v>41.4</v>
       </c>
+      <c r="AS132" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="B133" t="n">
         <v>51</v>
@@ -16938,7 +17336,7 @@
         <v>1</v>
       </c>
       <c r="AO133" t="n">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="AP133" t="n">
         <v>1</v>
@@ -16948,11 +17346,14 @@
       </c>
       <c r="AR133" t="n">
         <v>0</v>
+      </c>
+      <c r="AS133" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="B134" t="n">
         <v>52</v>
@@ -17075,10 +17476,13 @@
       <c r="AR134" t="n">
         <v>11.3</v>
       </c>
+      <c r="AS134" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="B135" t="n">
         <v>52</v>
@@ -17205,10 +17609,13 @@
       <c r="AR135" t="n">
         <v>50</v>
       </c>
+      <c r="AS135" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="B136" t="n">
         <v>52</v>
@@ -17323,10 +17730,13 @@
       <c r="AR136" t="n">
         <v>45</v>
       </c>
+      <c r="AS136" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="B137" t="n">
         <v>53</v>
@@ -17449,10 +17859,13 @@
       <c r="AR137" t="n">
         <v>41.3</v>
       </c>
+      <c r="AS137" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="B138" t="n">
         <v>53</v>
@@ -17575,10 +17988,13 @@
       <c r="AR138" t="n">
         <v>3.7</v>
       </c>
+      <c r="AS138" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="B139" t="n">
         <v>53</v>
@@ -17693,10 +18109,13 @@
       <c r="AR139" t="n">
         <v>0</v>
       </c>
+      <c r="AS139" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="B140" t="n">
         <v>54</v>
@@ -17728,7 +18147,7 @@
         <v>4</v>
       </c>
       <c r="M140" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="N140" t="n">
         <v>5</v>
@@ -17819,10 +18238,13 @@
       <c r="AR140" t="n">
         <v>19.2</v>
       </c>
+      <c r="AS140" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="B141" t="n">
         <v>54</v>
@@ -17945,10 +18367,13 @@
       <c r="AR141" t="n">
         <v>11</v>
       </c>
+      <c r="AS141" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="B142" t="n">
         <v>55</v>
@@ -18063,10 +18488,13 @@
       <c r="AR142" t="n">
         <v>4</v>
       </c>
+      <c r="AS142" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="B143" t="n">
         <v>55</v>
@@ -18189,10 +18617,13 @@
       <c r="AR143" t="n">
         <v>21</v>
       </c>
+      <c r="AS143" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="B144" t="n">
         <v>55</v>
@@ -18315,10 +18746,13 @@
       <c r="AR144" t="n">
         <v>30</v>
       </c>
+      <c r="AS144" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="B145" t="n">
         <v>56</v>
@@ -18441,10 +18875,13 @@
       <c r="AR145" t="n">
         <v>36.2</v>
       </c>
+      <c r="AS145" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="B146" t="n">
         <v>56</v>
@@ -18556,7 +18993,7 @@
         <v>1</v>
       </c>
       <c r="AO146" t="n">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="AP146" t="n">
         <v>1</v>
@@ -18566,11 +19003,14 @@
       </c>
       <c r="AR146" t="n">
         <v>5.1</v>
+      </c>
+      <c r="AS146" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="B147" t="n">
         <v>56</v>
@@ -18685,10 +19125,13 @@
       <c r="AR147" t="n">
         <v>10</v>
       </c>
+      <c r="AS147" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="B148" t="n">
         <v>57</v>
@@ -18811,10 +19254,13 @@
       <c r="AR148" t="n">
         <v>25</v>
       </c>
+      <c r="AS148" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="B149" t="n">
         <v>57</v>
@@ -18849,7 +19295,7 @@
         <v>5</v>
       </c>
       <c r="N149" t="n">
-        <v>-9</v>
+        <v>3</v>
       </c>
       <c r="O149" t="n">
         <v>2</v>
@@ -18929,6 +19375,1396 @@
       <c r="AR149" t="n">
         <v>75</v>
       </c>
+      <c r="AS149" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="n">
+        <v>58</v>
+      </c>
+      <c r="C150" t="n">
+        <v>2</v>
+      </c>
+      <c r="D150" t="n">
+        <v>3</v>
+      </c>
+      <c r="E150" t="n">
+        <v>1</v>
+      </c>
+      <c r="F150" t="n">
+        <v>8</v>
+      </c>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="n">
+        <v>3</v>
+      </c>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" t="n">
+        <v>5</v>
+      </c>
+      <c r="K150" t="n">
+        <v>4</v>
+      </c>
+      <c r="L150" t="n">
+        <v>5</v>
+      </c>
+      <c r="M150" t="n">
+        <v>2</v>
+      </c>
+      <c r="N150" t="n">
+        <v>4</v>
+      </c>
+      <c r="O150" t="n">
+        <v>3</v>
+      </c>
+      <c r="P150" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q150" t="n">
+        <v>2</v>
+      </c>
+      <c r="R150" t="n">
+        <v>1</v>
+      </c>
+      <c r="S150" t="n">
+        <v>4</v>
+      </c>
+      <c r="T150" t="inlineStr"/>
+      <c r="U150" t="inlineStr"/>
+      <c r="V150" t="n">
+        <v>29</v>
+      </c>
+      <c r="W150" t="n">
+        <v>71</v>
+      </c>
+      <c r="X150" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y150" t="n">
+        <v>69</v>
+      </c>
+      <c r="Z150" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA150" t="n">
+        <v>50</v>
+      </c>
+      <c r="AB150" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC150" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD150" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE150" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF150" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG150" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH150" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI150" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ150" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK150" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL150" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM150" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN150" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO150" t="n">
+        <v>388</v>
+      </c>
+      <c r="AP150" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ150" t="n">
+        <v>63.7</v>
+      </c>
+      <c r="AR150" t="n">
+        <v>36.3</v>
+      </c>
+      <c r="AS150" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="n">
+        <v>58</v>
+      </c>
+      <c r="C151" t="n">
+        <v>3</v>
+      </c>
+      <c r="D151" t="n">
+        <v>5</v>
+      </c>
+      <c r="E151" t="n">
+        <v>1</v>
+      </c>
+      <c r="F151" t="n">
+        <v>7</v>
+      </c>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="n">
+        <v>4</v>
+      </c>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="n">
+        <v>7</v>
+      </c>
+      <c r="K151" t="n">
+        <v>4</v>
+      </c>
+      <c r="L151" t="n">
+        <v>4</v>
+      </c>
+      <c r="M151" t="n">
+        <v>3</v>
+      </c>
+      <c r="N151" t="n">
+        <v>2</v>
+      </c>
+      <c r="O151" t="n">
+        <v>5</v>
+      </c>
+      <c r="P151" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q151" t="n">
+        <v>2</v>
+      </c>
+      <c r="R151" t="n">
+        <v>1</v>
+      </c>
+      <c r="S151" t="n">
+        <v>4</v>
+      </c>
+      <c r="T151" t="n">
+        <v>16</v>
+      </c>
+      <c r="U151" t="n">
+        <v>84</v>
+      </c>
+      <c r="V151" t="inlineStr"/>
+      <c r="W151" t="inlineStr"/>
+      <c r="X151" t="inlineStr"/>
+      <c r="Y151" t="inlineStr"/>
+      <c r="Z151" t="inlineStr"/>
+      <c r="AA151" t="inlineStr"/>
+      <c r="AB151" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC151" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD151" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE151" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF151" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG151" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH151" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI151" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ151" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK151" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL151" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM151" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN151" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO151" t="n">
+        <v>289</v>
+      </c>
+      <c r="AP151" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ151" t="n">
+        <v>84</v>
+      </c>
+      <c r="AR151" t="n">
+        <v>16</v>
+      </c>
+      <c r="AS151" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="n">
+        <v>59</v>
+      </c>
+      <c r="C152" t="n">
+        <v>3</v>
+      </c>
+      <c r="D152" t="n">
+        <v>3</v>
+      </c>
+      <c r="E152" t="n">
+        <v>2</v>
+      </c>
+      <c r="F152" t="n">
+        <v>8</v>
+      </c>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="n">
+        <v>3</v>
+      </c>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="n">
+        <v>5</v>
+      </c>
+      <c r="K152" t="n">
+        <v>2</v>
+      </c>
+      <c r="L152" t="n">
+        <v>5</v>
+      </c>
+      <c r="M152" t="n">
+        <v>4</v>
+      </c>
+      <c r="N152" t="n">
+        <v>1</v>
+      </c>
+      <c r="O152" t="n">
+        <v>2</v>
+      </c>
+      <c r="P152" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q152" t="n">
+        <v>2</v>
+      </c>
+      <c r="R152" t="n">
+        <v>1</v>
+      </c>
+      <c r="S152" t="n">
+        <v>5</v>
+      </c>
+      <c r="T152" t="n">
+        <v>26</v>
+      </c>
+      <c r="U152" t="n">
+        <v>74</v>
+      </c>
+      <c r="V152" t="inlineStr"/>
+      <c r="W152" t="inlineStr"/>
+      <c r="X152" t="inlineStr"/>
+      <c r="Y152" t="inlineStr"/>
+      <c r="Z152" t="inlineStr"/>
+      <c r="AA152" t="inlineStr"/>
+      <c r="AB152" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC152" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD152" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE152" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF152" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG152" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH152" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI152" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ152" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK152" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL152" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM152" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN152" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO152" t="n">
+        <v>325</v>
+      </c>
+      <c r="AP152" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ152" t="n">
+        <v>74</v>
+      </c>
+      <c r="AR152" t="n">
+        <v>26</v>
+      </c>
+      <c r="AS152" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="n">
+        <v>59</v>
+      </c>
+      <c r="C153" t="n">
+        <v>2</v>
+      </c>
+      <c r="D153" t="n">
+        <v>3</v>
+      </c>
+      <c r="E153" t="n">
+        <v>1</v>
+      </c>
+      <c r="F153" t="n">
+        <v>4</v>
+      </c>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="n">
+        <v>1</v>
+      </c>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" t="n">
+        <v>3</v>
+      </c>
+      <c r="K153" t="n">
+        <v>4</v>
+      </c>
+      <c r="L153" t="n">
+        <v>5</v>
+      </c>
+      <c r="M153" t="n">
+        <v>1</v>
+      </c>
+      <c r="N153" t="n">
+        <v>2</v>
+      </c>
+      <c r="O153" t="n">
+        <v>5</v>
+      </c>
+      <c r="P153" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q153" t="n">
+        <v>2</v>
+      </c>
+      <c r="R153" t="n">
+        <v>1</v>
+      </c>
+      <c r="S153" t="n">
+        <v>4</v>
+      </c>
+      <c r="T153" t="inlineStr"/>
+      <c r="U153" t="inlineStr"/>
+      <c r="V153" t="n">
+        <v>15</v>
+      </c>
+      <c r="W153" t="n">
+        <v>85</v>
+      </c>
+      <c r="X153" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y153" t="n">
+        <v>80</v>
+      </c>
+      <c r="Z153" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA153" t="n">
+        <v>89</v>
+      </c>
+      <c r="AB153" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC153" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD153" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE153" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF153" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG153" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH153" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI153" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ153" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK153" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL153" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM153" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN153" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO153" t="n">
+        <v>426</v>
+      </c>
+      <c r="AP153" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ153" t="n">
+        <v>83.7</v>
+      </c>
+      <c r="AR153" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="AS153" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="n">
+        <v>59</v>
+      </c>
+      <c r="C154" t="n">
+        <v>1</v>
+      </c>
+      <c r="D154" t="n">
+        <v>3</v>
+      </c>
+      <c r="E154" t="n">
+        <v>1</v>
+      </c>
+      <c r="F154" t="n">
+        <v>7</v>
+      </c>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="n">
+        <v>3</v>
+      </c>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" t="n">
+        <v>3</v>
+      </c>
+      <c r="K154" t="n">
+        <v>2</v>
+      </c>
+      <c r="L154" t="n">
+        <v>4</v>
+      </c>
+      <c r="M154" t="n">
+        <v>2</v>
+      </c>
+      <c r="N154" t="n">
+        <v>2</v>
+      </c>
+      <c r="O154" t="n">
+        <v>4</v>
+      </c>
+      <c r="P154" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q154" t="n">
+        <v>2</v>
+      </c>
+      <c r="R154" t="n">
+        <v>1</v>
+      </c>
+      <c r="S154" t="n">
+        <v>5</v>
+      </c>
+      <c r="T154" t="inlineStr"/>
+      <c r="U154" t="inlineStr"/>
+      <c r="V154" t="n">
+        <v>41</v>
+      </c>
+      <c r="W154" t="n">
+        <v>59</v>
+      </c>
+      <c r="X154" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y154" t="n">
+        <v>72</v>
+      </c>
+      <c r="Z154" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA154" t="n">
+        <v>68</v>
+      </c>
+      <c r="AB154" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC154" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD154" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE154" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF154" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG154" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH154" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI154" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ154" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK154" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL154" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM154" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN154" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO154" t="n">
+        <v>374</v>
+      </c>
+      <c r="AP154" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ154" t="n">
+        <v>69</v>
+      </c>
+      <c r="AR154" t="n">
+        <v>31</v>
+      </c>
+      <c r="AS154" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="n">
+        <v>60</v>
+      </c>
+      <c r="C155" t="n">
+        <v>2</v>
+      </c>
+      <c r="D155" t="n">
+        <v>4</v>
+      </c>
+      <c r="E155" t="n">
+        <v>1</v>
+      </c>
+      <c r="F155" t="n">
+        <v>7</v>
+      </c>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="n">
+        <v>3</v>
+      </c>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" t="n">
+        <v>4</v>
+      </c>
+      <c r="K155" t="n">
+        <v>4</v>
+      </c>
+      <c r="L155" t="n">
+        <v>4</v>
+      </c>
+      <c r="M155" t="n">
+        <v>3</v>
+      </c>
+      <c r="N155" t="n">
+        <v>5</v>
+      </c>
+      <c r="O155" t="n">
+        <v>4</v>
+      </c>
+      <c r="P155" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q155" t="n">
+        <v>2</v>
+      </c>
+      <c r="R155" t="n">
+        <v>1</v>
+      </c>
+      <c r="S155" t="n">
+        <v>5</v>
+      </c>
+      <c r="T155" t="inlineStr"/>
+      <c r="U155" t="inlineStr"/>
+      <c r="V155" t="n">
+        <v>16</v>
+      </c>
+      <c r="W155" t="n">
+        <v>84</v>
+      </c>
+      <c r="X155" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y155" t="n">
+        <v>82</v>
+      </c>
+      <c r="Z155" t="n">
+        <v>81</v>
+      </c>
+      <c r="AA155" t="n">
+        <v>19</v>
+      </c>
+      <c r="AB155" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC155" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD155" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE155" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF155" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG155" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH155" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI155" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ155" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK155" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL155" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM155" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN155" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO155" t="n">
+        <v>450</v>
+      </c>
+      <c r="AP155" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ155" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="AR155" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="AS155" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="n">
+        <v>60</v>
+      </c>
+      <c r="C156" t="n">
+        <v>1</v>
+      </c>
+      <c r="D156" t="n">
+        <v>3</v>
+      </c>
+      <c r="E156" t="n">
+        <v>2</v>
+      </c>
+      <c r="F156" t="n">
+        <v>8</v>
+      </c>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="n">
+        <v>3</v>
+      </c>
+      <c r="I156" t="inlineStr"/>
+      <c r="J156" t="n">
+        <v>5</v>
+      </c>
+      <c r="K156" t="n">
+        <v>4</v>
+      </c>
+      <c r="L156" t="n">
+        <v>4</v>
+      </c>
+      <c r="M156" t="n">
+        <v>3</v>
+      </c>
+      <c r="N156" t="n">
+        <v>4</v>
+      </c>
+      <c r="O156" t="n">
+        <v>3</v>
+      </c>
+      <c r="P156" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q156" t="n">
+        <v>2</v>
+      </c>
+      <c r="R156" t="n">
+        <v>1</v>
+      </c>
+      <c r="S156" t="n">
+        <v>4</v>
+      </c>
+      <c r="T156" t="inlineStr"/>
+      <c r="U156" t="inlineStr"/>
+      <c r="V156" t="n">
+        <v>0</v>
+      </c>
+      <c r="W156" t="n">
+        <v>100</v>
+      </c>
+      <c r="X156" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y156" t="n">
+        <v>100</v>
+      </c>
+      <c r="Z156" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA156" t="n">
+        <v>50</v>
+      </c>
+      <c r="AB156" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD156" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE156" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF156" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG156" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH156" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI156" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO156" t="n">
+        <v>242</v>
+      </c>
+      <c r="AP156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ156" t="n">
+        <v>95</v>
+      </c>
+      <c r="AR156" t="n">
+        <v>5</v>
+      </c>
+      <c r="AS156" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="n">
+        <v>60</v>
+      </c>
+      <c r="C157" t="n">
+        <v>3</v>
+      </c>
+      <c r="D157" t="n">
+        <v>4</v>
+      </c>
+      <c r="E157" t="n">
+        <v>1</v>
+      </c>
+      <c r="F157" t="n">
+        <v>8</v>
+      </c>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" t="n">
+        <v>3</v>
+      </c>
+      <c r="I157" t="inlineStr"/>
+      <c r="J157" t="n">
+        <v>1</v>
+      </c>
+      <c r="K157" t="n">
+        <v>3</v>
+      </c>
+      <c r="L157" t="n">
+        <v>4</v>
+      </c>
+      <c r="M157" t="n">
+        <v>2</v>
+      </c>
+      <c r="N157" t="n">
+        <v>2</v>
+      </c>
+      <c r="O157" t="n">
+        <v>4</v>
+      </c>
+      <c r="P157" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q157" t="n">
+        <v>2</v>
+      </c>
+      <c r="R157" t="n">
+        <v>1</v>
+      </c>
+      <c r="S157" t="n">
+        <v>2</v>
+      </c>
+      <c r="T157" t="n">
+        <v>30</v>
+      </c>
+      <c r="U157" t="n">
+        <v>70</v>
+      </c>
+      <c r="V157" t="inlineStr"/>
+      <c r="W157" t="inlineStr"/>
+      <c r="X157" t="inlineStr"/>
+      <c r="Y157" t="inlineStr"/>
+      <c r="Z157" t="inlineStr"/>
+      <c r="AA157" t="inlineStr"/>
+      <c r="AB157" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC157" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD157" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE157" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH157" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI157" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK157" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN157" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO157" t="n">
+        <v>361</v>
+      </c>
+      <c r="AP157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ157" t="n">
+        <v>70</v>
+      </c>
+      <c r="AR157" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS157" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="n">
+        <v>61</v>
+      </c>
+      <c r="C158" t="n">
+        <v>2</v>
+      </c>
+      <c r="D158" t="n">
+        <v>4</v>
+      </c>
+      <c r="E158" t="n">
+        <v>2</v>
+      </c>
+      <c r="F158" t="n">
+        <v>8</v>
+      </c>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="n">
+        <v>4</v>
+      </c>
+      <c r="I158" t="inlineStr"/>
+      <c r="J158" t="n">
+        <v>7</v>
+      </c>
+      <c r="K158" t="n">
+        <v>4</v>
+      </c>
+      <c r="L158" t="n">
+        <v>5</v>
+      </c>
+      <c r="M158" t="n">
+        <v>4</v>
+      </c>
+      <c r="N158" t="n">
+        <v>3</v>
+      </c>
+      <c r="O158" t="n">
+        <v>4</v>
+      </c>
+      <c r="P158" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q158" t="n">
+        <v>2</v>
+      </c>
+      <c r="R158" t="n">
+        <v>1</v>
+      </c>
+      <c r="S158" t="n">
+        <v>5</v>
+      </c>
+      <c r="T158" t="inlineStr"/>
+      <c r="U158" t="inlineStr"/>
+      <c r="V158" t="n">
+        <v>25</v>
+      </c>
+      <c r="W158" t="n">
+        <v>75</v>
+      </c>
+      <c r="X158" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y158" t="n">
+        <v>82</v>
+      </c>
+      <c r="Z158" t="n">
+        <v>70</v>
+      </c>
+      <c r="AA158" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF158" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG158" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ158" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN158" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO158" t="n">
+        <v>232</v>
+      </c>
+      <c r="AP158" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ158" t="n">
+        <v>65</v>
+      </c>
+      <c r="AR158" t="n">
+        <v>35</v>
+      </c>
+      <c r="AS158" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="n">
+        <v>61</v>
+      </c>
+      <c r="C159" t="n">
+        <v>3</v>
+      </c>
+      <c r="D159" t="n">
+        <v>7</v>
+      </c>
+      <c r="E159" t="n">
+        <v>1</v>
+      </c>
+      <c r="F159" t="n">
+        <v>8</v>
+      </c>
+      <c r="G159" t="inlineStr"/>
+      <c r="H159" t="n">
+        <v>4</v>
+      </c>
+      <c r="I159" t="inlineStr"/>
+      <c r="J159" t="n">
+        <v>8</v>
+      </c>
+      <c r="K159" t="n">
+        <v>4</v>
+      </c>
+      <c r="L159" t="n">
+        <v>5</v>
+      </c>
+      <c r="M159" t="n">
+        <v>4</v>
+      </c>
+      <c r="N159" t="n">
+        <v>2</v>
+      </c>
+      <c r="O159" t="n">
+        <v>4</v>
+      </c>
+      <c r="P159" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q159" t="n">
+        <v>2</v>
+      </c>
+      <c r="R159" t="n">
+        <v>1</v>
+      </c>
+      <c r="S159" t="n">
+        <v>4</v>
+      </c>
+      <c r="T159" t="n">
+        <v>20</v>
+      </c>
+      <c r="U159" t="n">
+        <v>80</v>
+      </c>
+      <c r="V159" t="inlineStr"/>
+      <c r="W159" t="inlineStr"/>
+      <c r="X159" t="inlineStr"/>
+      <c r="Y159" t="inlineStr"/>
+      <c r="Z159" t="inlineStr"/>
+      <c r="AA159" t="inlineStr"/>
+      <c r="AB159" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF159" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK159" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO159" t="n">
+        <v>330</v>
+      </c>
+      <c r="AP159" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ159" t="n">
+        <v>80</v>
+      </c>
+      <c r="AR159" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS159" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="n">
+        <v>61</v>
+      </c>
+      <c r="C160" t="n">
+        <v>1</v>
+      </c>
+      <c r="D160" t="n">
+        <v>4</v>
+      </c>
+      <c r="E160" t="n">
+        <v>2</v>
+      </c>
+      <c r="F160" t="n">
+        <v>7</v>
+      </c>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="n">
+        <v>4</v>
+      </c>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" t="n">
+        <v>7</v>
+      </c>
+      <c r="K160" t="n">
+        <v>4</v>
+      </c>
+      <c r="L160" t="n">
+        <v>5</v>
+      </c>
+      <c r="M160" t="n">
+        <v>4</v>
+      </c>
+      <c r="N160" t="n">
+        <v>4</v>
+      </c>
+      <c r="O160" t="n">
+        <v>3</v>
+      </c>
+      <c r="P160" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q160" t="n">
+        <v>2</v>
+      </c>
+      <c r="R160" t="n">
+        <v>1</v>
+      </c>
+      <c r="S160" t="n">
+        <v>5</v>
+      </c>
+      <c r="T160" t="inlineStr"/>
+      <c r="U160" t="inlineStr"/>
+      <c r="V160" t="n">
+        <v>16</v>
+      </c>
+      <c r="W160" t="n">
+        <v>84</v>
+      </c>
+      <c r="X160" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y160" t="n">
+        <v>81</v>
+      </c>
+      <c r="Z160" t="n">
+        <v>72</v>
+      </c>
+      <c r="AA160" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB160" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC160" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD160" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE160" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF160" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG160" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH160" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI160" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ160" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK160" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL160" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM160" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN160" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO160" t="n">
+        <v>301</v>
+      </c>
+      <c r="AP160" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ160" t="n">
+        <v>76.3</v>
+      </c>
+      <c r="AR160" t="n">
+        <v>23.7</v>
+      </c>
+      <c r="AS160" t="n">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>